<commit_message>
Improve aggregation of class properties
The code now checks for a lot more error conditions, and is able
to determine whether simple properties are nullable or not.

The code is a bit of a mess, but its all confined in a single class
</commit_message>
<xml_diff>
--- a/CustomerTestsExcel.Test/TestExcelFiles/VisitGivenComplexProperties.xlsx
+++ b/CustomerTestsExcel.Test/TestExcelFiles/VisitGivenComplexProperties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\Test\TestExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\CustomerTestsExcel.Test\TestExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{539665DD-E458-49B1-BE13-ADAF4987E61C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24CC598-803A-4EFD-AF5E-33624B2B7624}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="VisitGivenComplexProperties" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>When</t>
   </si>
   <si>
-    <t>Assert</t>
-  </si>
-  <si>
     <t>=</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>VisitGivenComplexProperties</t>
+  </si>
+  <si>
+    <t>Then</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -582,10 +582,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -596,10 +596,10 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -610,18 +610,18 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
       <c r="G9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -631,10 +631,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -642,23 +642,23 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>